<commit_message>
[FEAT(CriarNovoCliente)] - Arquitetura pagina novo cliente
</commit_message>
<xml_diff>
--- a/_docs/Burndown Sprint.xlsx
+++ b/_docs/Burndown Sprint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ProjetoGeral\Projeto_FestINF\_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ProjetoGeral\ProjetoMFI\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB5C41E-B4AF-44E2-BA13-BB9BF37C179C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D27608-3834-4A45-8BDF-9F022435BFAC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{0FB4B6D9-DE99-463B-91BE-0AC4D1FA3CA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FB4B6D9-DE99-463B-91BE-0AC4D1FA3CA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -411,28 +411,28 @@
                   <c:v>Total Estórias</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25/06/2019</c:v>
+                  <c:v>02/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>09/07/2019</c:v>
+                  <c:v>16/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/07/2019</c:v>
+                  <c:v>30/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>06/08/2019</c:v>
+                  <c:v>14/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20/08/2019</c:v>
+                  <c:v>28/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>03/09/2019</c:v>
+                  <c:v>11/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17/09/2019</c:v>
+                  <c:v>25/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>01/10/2019</c:v>
+                  <c:v>09/12/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -442,12 +442,9 @@
               <c:f>[0]!TotalEfetuado</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -494,28 +491,28 @@
                   <c:v>Total Estórias</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25/06/2019</c:v>
+                  <c:v>02/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>09/07/2019</c:v>
+                  <c:v>16/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/07/2019</c:v>
+                  <c:v>30/09/2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>06/08/2019</c:v>
+                  <c:v>14/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20/08/2019</c:v>
+                  <c:v>28/10/2019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>03/09/2019</c:v>
+                  <c:v>11/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17/09/2019</c:v>
+                  <c:v>25/11/2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>01/10/2019</c:v>
+                  <c:v>09/12/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1650,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A35631-EE6C-4E3F-BDC9-9183FE7D7F05}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,28 +1695,28 @@
         <v>9</v>
       </c>
       <c r="C2" s="8">
-        <v>43641</v>
+        <v>43710</v>
       </c>
       <c r="D2" s="8">
-        <v>43655</v>
+        <v>43724</v>
       </c>
       <c r="E2" s="8">
-        <v>43669</v>
+        <v>43738</v>
       </c>
       <c r="F2" s="8">
-        <v>43683</v>
+        <v>43752</v>
       </c>
       <c r="G2" s="8">
-        <v>43697</v>
+        <v>43766</v>
       </c>
       <c r="H2" s="8">
-        <v>43711</v>
+        <v>43780</v>
       </c>
       <c r="I2" s="8">
-        <v>43725</v>
+        <v>43794</v>
       </c>
       <c r="J2" s="9">
-        <v>43739</v>
+        <v>43808</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1729,9 +1726,7 @@
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="17">
-        <v>2</v>
-      </c>
+      <c r="C3" s="17"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1860,9 +1855,9 @@
         <f>SUM(B3:B10)</f>
         <v>29</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="15" t="str">
         <f>IF(SUM(C3:C10)&gt;0,B11-SUM(C3:C10),"")</f>
-        <v>27</v>
+        <v/>
       </c>
       <c r="D11" s="15" t="str">
         <f>IF(SUM(D3:D10)&gt;0,C11-SUM(D3:D10),"")</f>
@@ -1941,7 +1936,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1952,7 +1947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB25FC5-EF53-4859-8DF3-266EA3A5BA05}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[DOCS(*)] - ajuste de cronograma
</commit_message>
<xml_diff>
--- a/_docs/Burndown Sprint.xlsx
+++ b/_docs/Burndown Sprint.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ProjetoGeral\ProjetoMFI\_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workhome\ProjetoGeral\ProjetoMFI\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C339CFB9-0195-4200-97A5-69CA66703D39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FB4B6D9-DE99-463B-91BE-0AC4D1FA3CA1}"/>
+    <workbookView xWindow="-122" yWindow="-122" windowWidth="20731" windowHeight="11167" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="TotalEfetuado">OFFSET('Sprint 1'!$B$11,0,0,1,COUNT('Sprint 1'!$B$11:$J$11))</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +301,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -341,6 +340,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -442,18 +442,30 @@
               <c:f>[0]!TotalEfetuado</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BE8C-4567-A0FE-55ABF33C9185}"/>
             </c:ext>
@@ -557,7 +569,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-BE8C-4567-A0FE-55ABF33C9185}"/>
             </c:ext>
@@ -572,11 +584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1349792383"/>
-        <c:axId val="1412231663"/>
+        <c:axId val="344995768"/>
+        <c:axId val="344996160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1349792383"/>
+        <c:axId val="344995768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +631,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1412231663"/>
+        <c:crossAx val="344996160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -627,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1412231663"/>
+        <c:axId val="344996160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +690,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1349792383"/>
+        <c:crossAx val="344995768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -692,6 +704,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -723,14 +736,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1328,7 +1341,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC71104-622E-4E39-B65E-C09C18FE7835}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9AC71104-622E-4E39-B65E-C09C18FE7835}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1647,21 +1660,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A35631-EE6C-4E3F-BDC9-9183FE7D7F05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="10" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1690,7 +1703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1722,7 +1735,7 @@
         <v>43821</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1740,7 +1753,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1748,7 +1761,9 @@
         <v>4</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="18"/>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1756,7 +1771,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
@@ -1765,14 +1780,16 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="18"/>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1782,13 +1799,15 @@
       <c r="C6" s="4"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="18">
+        <v>1</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1799,12 +1818,14 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="18"/>
+      <c r="G7" s="18">
+        <v>1</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1820,7 +1841,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1836,7 +1857,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
@@ -1852,7 +1873,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="19"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
@@ -1864,21 +1885,21 @@
         <f>IF(SUM(C3:C10)&gt;0,B11-SUM(C3:C10),"")</f>
         <v>28</v>
       </c>
-      <c r="D11" s="15" t="str">
+      <c r="D11" s="15">
         <f>IF(SUM(D3:D10)&gt;0,C11-SUM(D3:D10),"")</f>
-        <v/>
-      </c>
-      <c r="E11" s="15" t="str">
+        <v>27</v>
+      </c>
+      <c r="E11" s="15">
         <f>IF(SUM(E3:E10)&gt;0,D11-SUM(E3:E10),"")</f>
-        <v/>
-      </c>
-      <c r="F11" s="15" t="str">
+        <v>26</v>
+      </c>
+      <c r="F11" s="15">
         <f t="shared" ref="F11:J11" si="0">IF(SUM(F3:F10)&gt;0,E11-SUM(F3:F10),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="15" t="str">
+        <v>25</v>
+      </c>
+      <c r="G11" s="15">
         <f t="shared" si="0"/>
-        <v/>
+        <v>24</v>
       </c>
       <c r="H11" s="15" t="str">
         <f t="shared" si="0"/>
@@ -1893,7 +1914,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>11</v>
       </c>
@@ -1949,14 +1970,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB25FC5-EF53-4859-8DF3-266EA3A5BA05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>